<commit_message>
Changed +5v pull ups in IoT BoM
</commit_message>
<xml_diff>
--- a/manufacture/BoM_RetroSpeechSynthIoTBoard.xlsx
+++ b/manufacture/BoM_RetroSpeechSynthIoTBoard.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="256">
   <si>
     <t>Source:</t>
   </si>
@@ -803,6 +803,9 @@
   </si>
   <si>
     <t>Order</t>
+  </si>
+  <si>
+    <t>4K7</t>
   </si>
 </sst>
 </file>
@@ -1157,9 +1160,9 @@
   <dimension ref="A1:L78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="900" activePane="bottomLeft"/>
+      <pane ySplit="900" topLeftCell="A19" activePane="bottomLeft"/>
       <selection activeCell="F4" sqref="F1:F1048576"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,7 +2567,7 @@
         <v>73</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
+        <v>255</v>
       </c>
       <c r="C43" t="s">
         <v>60</v>
@@ -2602,7 +2605,7 @@
         <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>59</v>
+        <v>255</v>
       </c>
       <c r="C44" t="s">
         <v>60</v>

</xml_diff>